<commit_message>
resolve date and time
</commit_message>
<xml_diff>
--- a/src/test/java/resources/data.xlsx
+++ b/src/test/java/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MySpace\DailyCode\Java\poidemo\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{93B3E055-D2BC-442C-B9A3-FF3FEF657A2C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A69F9DF3-59A0-46C6-9C64-9B3612C751B7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="7068" xr2:uid="{BAA7A24D-D08E-4DAA-A977-7C5D7CD148A7}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>成绩公示</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -118,6 +118,34 @@
   </si>
   <si>
     <t>黑罗伊</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>总分</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>平均分</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>日期</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>时间</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>排名（科学计数）</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖励（金钱）</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018.08.08</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -125,7 +153,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="3">
+    <numFmt numFmtId="176" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="177" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="178" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +190,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -180,7 +219,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -188,6 +227,24 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -510,25 +567,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0207466-FAB2-4AE5-BD23-69FA7FFB606B}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -547,8 +616,26 @@
       <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -567,8 +654,28 @@
       <c r="F3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f>SUM(C3:F3)</f>
+        <v>243</v>
+      </c>
+      <c r="H3">
+        <f>AVERAGE(C3:F3)</f>
+        <v>60.75</v>
+      </c>
+      <c r="I3" s="3">
+        <v>43320</v>
+      </c>
+      <c r="J3" s="4">
+        <v>0.67291666666666661</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1234</v>
+      </c>
+      <c r="L3" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -578,11 +685,31 @@
       <c r="C4">
         <v>90</v>
       </c>
+      <c r="E4">
+        <v>89</v>
+      </c>
       <c r="F4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" ref="G4:G8" si="0">SUM(C4:F4)</f>
+        <v>184</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H8" si="1">AVERAGE(C4:F4)</f>
+        <v>61.333333333333336</v>
+      </c>
+      <c r="I4" s="5">
+        <v>43320</v>
+      </c>
+      <c r="J4" s="4">
+        <v>0.71460648148148154</v>
+      </c>
+      <c r="L4" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -595,22 +722,50 @@
       <c r="F5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="4">
+        <v>0.75627314814814794</v>
+      </c>
+      <c r="L5" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
-        <v>60</v>
+      <c r="E6">
+        <v>25</v>
       </c>
       <c r="F6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="4">
+        <v>0.79793981481481502</v>
+      </c>
+      <c r="L6" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -620,11 +775,27 @@
       <c r="C7">
         <v>90</v>
       </c>
+      <c r="D7">
+        <v>65</v>
+      </c>
       <c r="F7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>53.333333333333336</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="7">
+        <v>1238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -637,13 +808,31 @@
       <c r="F8">
         <v>4</v>
       </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
+      </c>
+      <c r="I8" s="6">
+        <v>43322</v>
+      </c>
+      <c r="J8" s="4">
+        <v>0.88127314814814794</v>
+      </c>
+      <c r="K8" s="7">
+        <v>1239</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -702,15 +891,15 @@
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
resolve sheet by sheet name
</commit_message>
<xml_diff>
--- a/src/test/java/resources/data.xlsx
+++ b/src/test/java/resources/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MySpace\DailyCode\Java\poidemo\src\test\java\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{A69F9DF3-59A0-46C6-9C64-9B3612C751B7}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E896633-30A8-435D-9F5A-4F9DD035552A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="7068" xr2:uid="{BAA7A24D-D08E-4DAA-A977-7C5D7CD148A7}"/>
   </bookViews>
@@ -570,7 +570,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD6"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>

</xml_diff>